<commit_message>
Add generated Export.xlsx to root directory
</commit_message>
<xml_diff>
--- a/Export.xlsx
+++ b/Export.xlsx
@@ -1183,9 +1183,9 @@
           <t>OFF</t>
         </is>
       </c>
-      <c r="D21" s="6" t="inlineStr">
-        <is>
-          <t>OFF</t>
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>9:30AM-4PM</t>
         </is>
       </c>
       <c r="E21" s="4" t="inlineStr">
@@ -1225,9 +1225,9 @@
           <t>9:30AM-4PM</t>
         </is>
       </c>
-      <c r="D22" s="4" t="inlineStr">
-        <is>
-          <t>9:30AM-4PM</t>
+      <c r="D22" s="6" t="inlineStr">
+        <is>
+          <t>OFF</t>
         </is>
       </c>
       <c r="E22" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Add new generated Export.xlsx
</commit_message>
<xml_diff>
--- a/Export.xlsx
+++ b/Export.xlsx
@@ -716,9 +716,9 @@
           <t>OFF</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>9:45AM-4PM</t>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D8" s="6" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="C12" s="4" t="inlineStr">
         <is>
-          <t>9:30AM-4PM</t>
+          <t>9:45AM-4PM</t>
         </is>
       </c>
       <c r="D12" s="6" t="inlineStr">
@@ -982,9 +982,9 @@
           <t>10AM-5PM</t>
         </is>
       </c>
-      <c r="C15" s="6" t="inlineStr">
-        <is>
-          <t>OFF</t>
+      <c r="C15" s="4" t="inlineStr">
+        <is>
+          <t>10AM-5PM</t>
         </is>
       </c>
       <c r="D15" s="4" t="inlineStr">
@@ -1024,9 +1024,9 @@
           <t>OFF</t>
         </is>
       </c>
-      <c r="C16" s="4" t="inlineStr">
-        <is>
-          <t>10AM-5PM</t>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D16" s="6" t="inlineStr">
@@ -1323,46 +1323,52 @@
       </c>
       <c r="C27" s="7" t="inlineStr">
         <is>
+          <t>Lifeguard,
+9:30AM-4PM</t>
+        </is>
+      </c>
+      <c r="D27" s="7" t="inlineStr">
+        <is>
+          <t>Lifeguard,
+9:30AM-4PM</t>
+        </is>
+      </c>
+      <c r="E27" s="7" t="inlineStr">
+        <is>
+          <t>PA,
+10AM-5PM</t>
+        </is>
+      </c>
+      <c r="F27" s="7" t="inlineStr">
+        <is>
+          <t>Lifeguard,
+9:45AM-5PM</t>
+        </is>
+      </c>
+      <c r="G27" s="7" t="inlineStr">
+        <is>
+          <t>Lifeguard,
+9:45AM-5PM</t>
+        </is>
+      </c>
+      <c r="H27" s="7" t="inlineStr">
+        <is>
+          <t>Lifeguard,
+9:30AM-5PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="7" t="inlineStr">
+        <is>
+          <t>Lifeguard,
+9:30AM-4PM</t>
+        </is>
+      </c>
+      <c r="C28" s="7" t="inlineStr">
+        <is>
           <t>Bartender,
 10AM-4PM</t>
-        </is>
-      </c>
-      <c r="D27" s="7" t="inlineStr">
-        <is>
-          <t>Lifeguard,
-9:30AM-4PM</t>
-        </is>
-      </c>
-      <c r="E27" s="7" t="inlineStr">
-        <is>
-          <t>PA,
-10AM-5PM</t>
-        </is>
-      </c>
-      <c r="F27" s="7" t="inlineStr">
-        <is>
-          <t>Lifeguard,
-9:45AM-5PM</t>
-        </is>
-      </c>
-      <c r="G27" s="7" t="inlineStr">
-        <is>
-          <t>Lifeguard,
-9:45AM-5PM</t>
-        </is>
-      </c>
-      <c r="H27" s="7" t="inlineStr">
-        <is>
-          <t>Lifeguard,
-9:30AM-5PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="7" t="inlineStr">
-        <is>
-          <t>Lifeguard,
-9:30AM-4PM</t>
         </is>
       </c>
       <c r="E28" s="7" t="inlineStr">

</xml_diff>